<commit_message>
Realizando auditoria da PSI - XPTO
Signed-off-by: Marcos Aurélio <marcosaurelio88@gmail.com>
</commit_message>
<xml_diff>
--- a/PSI/Auditoria PSI.xlsx
+++ b/PSI/Auditoria PSI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoDrive\Pós Estácio\Sistema de Geestão de Segurança da Informação\Estudo de caso - XPTO\xpto\PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D718F3AC-B86F-4EB0-981B-D308C769F3BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEC5B50-8661-478F-8A39-F4F5A3E04533}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{D02F8A75-6682-4885-B874-A9F569CFD882}"/>
   </bookViews>
@@ -796,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -821,21 +821,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -845,9 +836,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -863,6 +851,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -883,6 +874,57 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1200,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3AFA5D-6481-4296-8012-4729C08E7497}">
   <dimension ref="A2:N201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B181" workbookViewId="0">
-      <selection activeCell="C191" sqref="C191:C195"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1248,7 +1290,7 @@
       <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="25" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="7"/>
@@ -1266,7 +1308,7 @@
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="32" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="6"/>
@@ -1284,7 +1326,7 @@
       <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="32" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
@@ -1302,7 +1344,7 @@
       <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="6"/>
@@ -1320,22 +1362,22 @@
       <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="34" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="34" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="35" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1343,7 +1385,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1351,7 +1393,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="34" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1359,7 +1401,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="35" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1367,7 +1409,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="35" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1375,87 +1417,87 @@
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="34" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="35" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="37" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="34" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="34" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="35" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="34" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="35" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="34" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="35" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="34" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="36" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1471,32 +1513,32 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="30" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="12" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1509,7 +1551,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="13" t="s">
         <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -1517,7 +1559,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="31" t="s">
         <v>47</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -1525,7 +1567,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="31" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -1533,7 +1575,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="31" t="s">
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -1541,51 +1583,51 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="44" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="44" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="44" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="20" t="s">
+      <c r="A55" s="45" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="45" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="45" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="46" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="26" t="s">
+      <c r="A63" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C63" s="21"/>
+      <c r="C63" s="17"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
@@ -1604,7 +1646,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="18" t="s">
         <v>60</v>
       </c>
       <c r="C66" s="4" t="s">
@@ -1612,7 +1654,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="38" t="s">
         <v>61</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -1620,7 +1662,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="38" t="s">
         <v>62</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -1628,62 +1670,62 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="38" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="19" t="s">
+      <c r="A70" s="38" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="19" t="s">
+      <c r="A71" s="38" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="38" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="19" t="s">
+      <c r="A73" s="43" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="38" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="22" t="s">
+      <c r="A75" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="19" t="s">
+      <c r="A76" s="38" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="38" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="19" t="s">
+      <c r="A78" s="38" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="38" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
+      <c r="A80" s="38" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1698,102 +1740,102 @@
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="24" t="s">
+      <c r="A83" s="20" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A84" s="25" t="s">
+      <c r="A84" s="21" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="25" t="s">
+      <c r="A85" s="39" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="25" t="s">
+      <c r="A86" s="39" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="24" t="s">
+      <c r="A87" s="20" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A88" s="25" t="s">
+      <c r="A88" s="21" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A89" s="25" t="s">
+      <c r="A89" s="21" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A90" s="25" t="s">
+      <c r="A90" s="21" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" s="25" t="s">
+      <c r="A91" s="40" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A92" s="25" t="s">
+      <c r="A92" s="21" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A93" s="25" t="s">
+      <c r="A93" s="21" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" s="24" t="s">
+      <c r="A94" s="20" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A95" s="25" t="s">
+      <c r="A95" s="41" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A96" s="25" t="s">
+      <c r="A96" s="39" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="25" t="s">
+      <c r="A97" s="41" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" s="27" t="s">
+      <c r="A98" s="24" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" s="28" t="s">
+      <c r="A99" s="25" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="25" t="s">
+      <c r="A100" s="39" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="25" t="s">
+      <c r="A101" s="41" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="25" t="s">
+      <c r="A102" s="39" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1808,414 +1850,414 @@
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="27" t="s">
+      <c r="A105" s="24" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="25" t="s">
+      <c r="A106" s="39" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="25" t="s">
+      <c r="A107" s="41" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108" s="25" t="s">
+      <c r="A108" s="42" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A109" s="25" t="s">
+      <c r="A109" s="39" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110" s="25" t="s">
+      <c r="A110" s="21" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="29" t="s">
+      <c r="A111" s="26" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="116" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="26" t="s">
+    <row r="115" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C116" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C117" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C118" s="30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" s="27" t="s">
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="C119" s="31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A120" s="25" t="s">
+    </row>
+    <row r="120" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A120" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C120" s="32" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A121" s="25" t="s">
+    </row>
+    <row r="121" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A121" s="21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A122" s="25" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="21" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" s="25" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" s="21" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" s="25" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="21" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" s="27" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" s="24" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A126" s="25" t="s">
+    <row r="126" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A126" s="21" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="127" spans="1:3" s="23" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A127" s="25" t="s">
+    <row r="127" spans="1:1" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A127" s="21" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" s="25" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" s="21" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A129" s="25" t="s">
+      <c r="A129" s="21" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A130" s="25" t="s">
+      <c r="A130" s="21" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A131" s="27" t="s">
+      <c r="A131" s="24" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A132" s="25" t="s">
+      <c r="A132" s="21" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A133" s="25" t="s">
+      <c r="A133" s="21" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134" s="27" t="s">
+      <c r="A134" s="24" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A135" s="25" t="s">
+      <c r="A135" s="21" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136" s="27" t="s">
+      <c r="A136" s="24" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A137" s="25" t="s">
+      <c r="A137" s="21" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A138" s="25" t="s">
+      <c r="A138" s="21" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A139" s="25" t="s">
+      <c r="A139" s="21" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A140" s="25" t="s">
+      <c r="A140" s="21" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A141" s="27" t="s">
+      <c r="A141" s="24" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A142" s="25" t="s">
+      <c r="A142" s="21" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A143" s="25" t="s">
+      <c r="A143" s="21" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="25" t="s">
+      <c r="A144" s="21" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="146" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A146" s="10" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A147" s="27" t="s">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A148" s="25" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="21" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A149" s="25" t="s">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" s="21" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A150" s="25" t="s">
+    <row r="150" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A150" s="21" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A151" s="27" t="s">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" s="24" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A152" s="25" t="s">
+      <c r="C151" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" s="21" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A153" s="25" t="s">
+      <c r="C152" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" s="21" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A154" s="25" t="s">
+      <c r="C153" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" s="21" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A155" s="25" t="s">
+      <c r="C154" s="28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" s="21" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A156" s="25" t="s">
+      <c r="C155" s="29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" s="21" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A157" s="27" t="s">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" s="24" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A158" s="25" t="s">
+    <row r="158" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A158" s="21" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A159" s="25" t="s">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A160" s="25" t="s">
+    <row r="160" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A160" s="21" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A161" s="27" t="s">
+      <c r="A161" s="24" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A162" s="25" t="s">
+      <c r="A162" s="21" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A163" s="25" t="s">
+      <c r="A163" s="21" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A164" s="25" t="s">
+      <c r="A164" s="21" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A165" s="25" t="s">
+      <c r="A165" s="21" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A166" s="25" t="s">
+      <c r="A166" s="21" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A167" s="25" t="s">
+      <c r="A167" s="21" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A168" s="27" t="s">
+      <c r="A168" s="24" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A169" s="25" t="s">
+      <c r="A169" s="21" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A170" s="25" t="s">
+      <c r="A170" s="21" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A171" s="25" t="s">
+      <c r="A171" s="21" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A172" s="27" t="s">
+      <c r="A172" s="24" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A173" s="25" t="s">
+      <c r="A173" s="21" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="174" spans="1:1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A174" s="25" t="s">
+      <c r="A174" s="21" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="175" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A175" s="25" t="s">
+      <c r="A175" s="21" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A176" s="27" t="s">
+      <c r="A176" s="24" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A177" s="25" t="s">
+      <c r="A177" s="21" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A178" s="25" t="s">
+      <c r="A178" s="21" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A179" s="25" t="s">
+      <c r="A179" s="21" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A180" s="27" t="s">
+      <c r="A180" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A181" s="25" t="s">
+      <c r="A181" s="21" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A182" s="25" t="s">
+      <c r="A182" s="21" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A183" s="25" t="s">
+      <c r="A183" s="21" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A184" s="27" t="s">
+      <c r="A184" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A185" s="25" t="s">
+      <c r="A185" s="21" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="29" t="s">
+      <c r="A186" s="26" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="191" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="26" t="s">
+      <c r="A191" s="23" t="s">
         <v>177</v>
       </c>
       <c r="C191" s="5" t="s">
@@ -2231,56 +2273,56 @@
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A193" s="27" t="s">
+      <c r="A193" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="C193" s="30" t="s">
+      <c r="C193" s="27" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A194" s="25" t="s">
+      <c r="A194" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C194" s="31" t="s">
+      <c r="C194" s="28" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A195" s="25" t="s">
+      <c r="A195" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="C195" s="32" t="s">
+      <c r="C195" s="29" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A196" s="25" t="s">
+      <c r="A196" s="21" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A197" s="25" t="s">
+      <c r="A197" s="21" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A198" s="25" t="s">
+      <c r="A198" s="21" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A199" s="25" t="s">
+      <c r="A199" s="21" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A200" s="25" t="s">
+      <c r="A200" s="21" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="29" t="s">
+      <c r="A201" s="26" t="s">
         <v>187</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Avaliação de Ites da XPTO e disponibilização do modelo de Auditoria PSI - Modelo.xlsx, que deve ser alterado para auditorias futuras.
Signed-off-by: Marcos Aurélio <marcosaurelio88@gmail.com>
</commit_message>
<xml_diff>
--- a/PSI/Auditoria PSI.xlsx
+++ b/PSI/Auditoria PSI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoDrive\Pós Estácio\Sistema de Geestão de Segurança da Informação\Estudo de caso - XPTO\xpto\PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEC5B50-8661-478F-8A39-F4F5A3E04533}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EACC6FB-BDCB-4120-9EA7-AA9F5C975417}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{D02F8A75-6682-4885-B874-A9F569CFD882}"/>
   </bookViews>
@@ -33,12 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="188">
   <si>
-    <t>Mapeamento dos incidentes que violam as regras da PSI</t>
-  </si>
-  <si>
-    <t>Analise critica em intervalos planejados ou quando mudanças significativas ocorrerem</t>
-  </si>
-  <si>
     <t>Analise critica da POLÍTICA DE SEGURANÇA DA INFORMAÇÃO</t>
   </si>
   <si>
@@ -471,9 +465,6 @@
     <t>Seja alarmada para detectar mal funcionamento, quando necessário;</t>
   </si>
   <si>
-    <t>Tenham múltiplas alimentações com rotas físicas diferentes;</t>
-  </si>
-  <si>
     <t>11.2.3 Segurança do cabeamento</t>
   </si>
   <si>
@@ -595,6 +586,15 @@
   </si>
   <si>
     <t>Provisão de um processo emergencial de mudança para permitir uma implementação rápida e controlada de mudanças, necessárias para resolver um incidente (ver 16.1).</t>
+  </si>
+  <si>
+    <t>Mapeamento dos incidentes que violam as regras da PSI.</t>
+  </si>
+  <si>
+    <t>Analise critica em intervalos planejados ou quando mudanças significativas ocorrerem;</t>
+  </si>
+  <si>
+    <t>Tenham múltiplas alimentações com rotas físicas diferentes.</t>
   </si>
 </sst>
 </file>
@@ -796,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -820,22 +820,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -848,9 +838,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -863,9 +850,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -884,30 +868,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -925,6 +894,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1242,20 +1233,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3AFA5D-6481-4296-8012-4729C08E7497}">
   <dimension ref="A2:N201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="150.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="150.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1273,7 +1264,7 @@
     </row>
     <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1290,8 +1281,8 @@
       <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
-        <v>33</v>
+      <c r="A5" s="20" t="s">
+        <v>31</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1308,8 +1299,8 @@
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
-        <v>32</v>
+      <c r="A6" s="26" t="s">
+        <v>30</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1326,8 +1317,8 @@
       <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
-        <v>31</v>
+      <c r="A7" s="26" t="s">
+        <v>29</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1344,8 +1335,8 @@
       <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
-        <v>30</v>
+      <c r="A8" s="36" t="s">
+        <v>28</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1362,968 +1353,968 @@
       <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
-        <v>29</v>
+      <c r="A9" s="17" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
-        <v>28</v>
+      <c r="A10" s="27" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="34" t="s">
-        <v>27</v>
+      <c r="A11" s="27" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="35" t="s">
-        <v>26</v>
+      <c r="A12" s="41" t="s">
+        <v>24</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
-        <v>24</v>
+      <c r="A13" s="17" t="s">
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="34" t="s">
-        <v>22</v>
+      <c r="A14" s="27" t="s">
+        <v>20</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="35" t="s">
-        <v>20</v>
+      <c r="A15" s="41" t="s">
+        <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
-        <v>18</v>
+      <c r="A16" s="27" t="s">
+        <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
-        <v>16</v>
+      <c r="A17" s="17" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34" t="s">
-        <v>15</v>
+      <c r="A18" s="27" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
-        <v>14</v>
+      <c r="A19" s="43" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37" t="s">
-        <v>13</v>
+      <c r="A20" s="41" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="34" t="s">
-        <v>12</v>
+      <c r="A21" s="27" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="34" t="s">
-        <v>11</v>
+      <c r="A22" s="27" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="34" t="s">
-        <v>10</v>
+      <c r="A23" s="27" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="35" t="s">
-        <v>9</v>
+      <c r="A24" s="41" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="34" t="s">
-        <v>8</v>
+      <c r="A25" s="27" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="34" t="s">
-        <v>7</v>
+      <c r="A26" s="27" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="34" t="s">
-        <v>6</v>
+      <c r="A27" s="27" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="35" t="s">
-        <v>5</v>
+      <c r="A28" s="41" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="34" t="s">
-        <v>4</v>
+      <c r="A29" s="27" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="35" t="s">
-        <v>3</v>
+      <c r="A30" s="43" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="22" t="s">
-        <v>2</v>
+      <c r="A31" s="17" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="34" t="s">
-        <v>1</v>
+      <c r="A32" s="27" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
-        <v>0</v>
+      <c r="A33" s="42" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="15" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="30" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="12" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="38" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="12" t="s">
+      <c r="C46" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
+      <c r="C47" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="31" t="s">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="44" t="s">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="34" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="44" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="44" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="34" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="45" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="34" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="45" t="s">
+    <row r="58" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="35" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="45" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="46" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C63" s="17"/>
+      <c r="A63" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="13"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="18" t="s">
+      <c r="A66" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="38" t="s">
+      <c r="C68" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="38" t="s">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="38" t="s">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="28" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="38" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="28" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="38" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="32" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="38" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="28" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="43" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="38" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="38" t="s">
+      <c r="A76" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="28" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="38" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="38" t="s">
+    <row r="80" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="28" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="38" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="20" t="s">
-        <v>72</v>
-      </c>
-    </row>
     <row r="84" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A84" s="21" t="s">
+      <c r="A84" s="30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="29" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="39" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="39" t="s">
+    <row r="88" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A88" s="30" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="20" t="s">
+    <row r="89" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A89" s="30" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A88" s="21" t="s">
+    <row r="90" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A90" s="30" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A89" s="21" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="30" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A90" s="21" t="s">
+    <row r="92" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A92" s="30" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" s="40" t="s">
+    <row r="93" spans="1:1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A93" s="30" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A92" s="21" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A93" s="21" t="s">
+    <row r="95" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A95" s="29" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" s="20" t="s">
+    <row r="96" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A96" s="29" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A95" s="41" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="30" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A96" s="39" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="41" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="20" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" s="24" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="29" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" s="25" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="30" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="39" t="s">
+    <row r="102" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="29" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="39" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="24" t="s">
+      <c r="A105" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="39" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="31" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="41" t="s">
+    <row r="109" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A109" s="29" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108" s="42" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="29" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A109" s="39" t="s">
+    <row r="111" spans="1:1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="37" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110" s="21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="26" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="116" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="23" t="s">
-        <v>133</v>
+      <c r="A116" s="18" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A120" s="29" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" s="24" t="s">
+    <row r="121" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A121" s="31" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A120" s="21" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="29" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A121" s="21" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" s="29" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A122" s="21" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="29" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A123" s="21" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" s="19" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A124" s="21" t="s">
+    <row r="126" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A126" s="29" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A125" s="24" t="s">
+    <row r="127" spans="1:1" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A127" s="29" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A126" s="21" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" s="30" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="127" spans="1:1" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A127" s="21" t="s">
+    <row r="129" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A129" s="29" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A128" s="21" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" s="31" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="129" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A129" s="21" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="19" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A130" s="21" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="29" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A131" s="24" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="29" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A132" s="21" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="19" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A133" s="21" t="s">
+    <row r="135" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A135" s="31" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134" s="24" t="s">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="19" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="135" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A135" s="21" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="31" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136" s="24" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="29" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A137" s="21" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="29" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A138" s="21" t="s">
+    <row r="140" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A140" s="31" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A139" s="21" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" s="19" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="140" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A140" s="21" t="s">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" s="30" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A141" s="24" t="s">
+    <row r="143" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A143" s="30" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A142" s="21" t="s">
+    <row r="144" spans="1:1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="30" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A143" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="21" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A146" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="19" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A147" s="24" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" s="29" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A148" s="21" t="s">
+    <row r="150" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A150" s="30" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A149" s="21" t="s">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" s="19" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A150" s="21" t="s">
+      <c r="C151" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" s="30" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A151" s="24" t="s">
+      <c r="C152" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="C151" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A152" s="21" t="s">
+      <c r="C153" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="C152" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A153" s="21" t="s">
+      <c r="C154" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="C153" s="27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A154" s="21" t="s">
+      <c r="C155" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" s="30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="C154" s="28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A155" s="21" t="s">
+    </row>
+    <row r="158" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A158" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="C155" s="29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A156" s="21" t="s">
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" s="30" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A157" s="24" t="s">
+    <row r="160" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A160" s="30" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A158" s="21" t="s">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" s="19" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A159" s="21" t="s">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" s="31" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A160" s="21" t="s">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" s="30" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A161" s="24" t="s">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" s="30" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A162" s="21" t="s">
+    <row r="165" spans="1:1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A165" s="29" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A163" s="21" t="s">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" s="30" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A164" s="21" t="s">
+    <row r="167" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A167" s="30" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="165" spans="1:1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A165" s="21" t="s">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" s="19" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A166" s="21" t="s">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" s="30" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="167" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A167" s="21" t="s">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" s="30" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A168" s="24" t="s">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" s="30" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A169" s="21" t="s">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" s="19" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A170" s="21" t="s">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" s="30" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A171" s="21" t="s">
+    <row r="174" spans="1:1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A174" s="30" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A172" s="24" t="s">
+    <row r="175" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A175" s="30" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A173" s="21" t="s">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" s="19" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="174" spans="1:1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A174" s="21" t="s">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" s="30" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="175" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A175" s="21" t="s">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" s="30" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A176" s="24" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" s="30" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A177" s="21" t="s">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" s="19" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A178" s="21" t="s">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" s="30" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A179" s="21" t="s">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" s="30" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A180" s="24" t="s">
+    <row r="183" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A183" s="30" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A181" s="21" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" s="19" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A182" s="21" t="s">
+    <row r="185" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A185" s="30" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A183" s="21" t="s">
+    <row r="186" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="37" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A184" s="24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A185" s="21" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="26" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="191" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="23" t="s">
-        <v>177</v>
+      <c r="A191" s="18" t="s">
+        <v>174</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A192" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C192" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C193" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C194" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="C192" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A193" s="24" t="s">
+      <c r="C195" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="C193" s="27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A194" s="21" t="s">
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="C194" s="28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A195" s="21" t="s">
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="C195" s="29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A196" s="21" t="s">
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" s="31" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A197" s="21" t="s">
+    <row r="200" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A200" s="30" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A198" s="21" t="s">
+    <row r="201" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="37" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A199" s="21" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A200" s="21" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="26" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>